<commit_message>
Updated for first release
</commit_message>
<xml_diff>
--- a/images/laplace.xlsx
+++ b/images/laplace.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12510" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12510"/>
   </bookViews>
   <sheets>
     <sheet name="Jacobi" sheetId="1" r:id="rId1"/>
@@ -252,7 +252,7 @@
                   <c:v>20.732638000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.9932409999999998</c:v>
+                  <c:v>74.480391999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>145.76655199999999</c:v>
@@ -274,12 +274,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="125617168"/>
-        <c:axId val="126272344"/>
+        <c:axId val="157089536"/>
+        <c:axId val="157214664"/>
         <c:extLst/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="125617168"/>
+        <c:axId val="157089536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -322,7 +322,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="126272344"/>
+        <c:crossAx val="157214664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -330,7 +330,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126272344"/>
+        <c:axId val="157214664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -442,7 +442,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="125617168"/>
+        <c:crossAx val="157089536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -454,38 +454,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -645,7 +613,7 @@
                   <c:v>20.732638000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.6242499999999995</c:v>
+                  <c:v>3.6145690000000004</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>3.4975609999999997</c:v>
@@ -726,7 +694,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="9">
-                  <c:v>2.7458E-2</c:v>
+                  <c:v>34.382899999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>46.704880000000003</c:v>
@@ -807,7 +775,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="9" formatCode="0.00">
-                  <c:v>0.34153300000000009</c:v>
+                  <c:v>36.482922999999992</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00">
                   <c:v>95.564110999999997</c:v>
@@ -826,11 +794,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="125425744"/>
-        <c:axId val="393744200"/>
+        <c:axId val="116107824"/>
+        <c:axId val="116108216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="125425744"/>
+        <c:axId val="116107824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -873,7 +841,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="393744200"/>
+        <c:crossAx val="116108216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -881,7 +849,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="393744200"/>
+        <c:axId val="116108216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -988,7 +956,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="125425744"/>
+        <c:crossAx val="116107824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1237,8 +1205,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="146106000"/>
-        <c:axId val="391512808"/>
+        <c:axId val="116109000"/>
+        <c:axId val="116109392"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -1344,7 +1312,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="146106000"/>
+        <c:axId val="116109000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1387,7 +1355,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="391512808"/>
+        <c:crossAx val="116109392"/>
         <c:crossesAt val="1"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1395,7 +1363,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="391512808"/>
+        <c:axId val="116109392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1446,7 +1414,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146106000"/>
+        <c:crossAx val="116109000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1676,11 +1644,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="391514768"/>
-        <c:axId val="391514376"/>
+        <c:axId val="157529536"/>
+        <c:axId val="157529928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="391514768"/>
+        <c:axId val="157529536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1723,7 +1691,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="391514376"/>
+        <c:crossAx val="157529928"/>
         <c:crossesAt val="1"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1731,7 +1699,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="391514376"/>
+        <c:axId val="157529928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1782,7 +1750,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="391514768"/>
+        <c:crossAx val="157529536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4402,8 +4370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4443,7 +4411,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1">
-        <f>B2</f>
+        <f t="shared" ref="F2:F10" si="0">B2</f>
         <v>92.060850000000002</v>
       </c>
     </row>
@@ -4458,7 +4426,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1">
-        <f>B3</f>
+        <f t="shared" si="0"/>
         <v>45.444941</v>
       </c>
     </row>
@@ -4473,7 +4441,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1">
-        <f>B4</f>
+        <f t="shared" si="0"/>
         <v>26.129261</v>
       </c>
     </row>
@@ -4488,7 +4456,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1">
-        <f>B5</f>
+        <f t="shared" si="0"/>
         <v>21.354685</v>
       </c>
     </row>
@@ -4503,7 +4471,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1">
-        <f>B6</f>
+        <f t="shared" si="0"/>
         <v>20.810041999999999</v>
       </c>
     </row>
@@ -4518,7 +4486,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1">
-        <f>B7</f>
+        <f t="shared" si="0"/>
         <v>20.577961999999999</v>
       </c>
     </row>
@@ -4533,7 +4501,7 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1">
-        <f>B8</f>
+        <f t="shared" si="0"/>
         <v>20.495215000000002</v>
       </c>
     </row>
@@ -4548,7 +4516,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1">
-        <f>B9</f>
+        <f t="shared" si="0"/>
         <v>21.918222</v>
       </c>
     </row>
@@ -4563,7 +4531,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1">
-        <f>B10</f>
+        <f t="shared" si="0"/>
         <v>20.732638000000001</v>
       </c>
     </row>
@@ -4572,25 +4540,25 @@
         <v>1</v>
       </c>
       <c r="B11" s="1">
-        <v>3.9932409999999998</v>
+        <v>74.480391999999995</v>
       </c>
       <c r="C11" s="1">
-        <v>1.4478E-2</v>
+        <v>22.91516</v>
       </c>
       <c r="D11" s="1">
-        <v>1.298E-2</v>
+        <v>11.467739999999999</v>
       </c>
       <c r="E11" s="1">
         <f>C11+D11</f>
-        <v>2.7458E-2</v>
+        <v>34.382899999999999</v>
       </c>
       <c r="F11" s="1">
-        <f>2.172296+1.231512+0.220442</f>
-        <v>3.6242499999999995</v>
+        <f>2.160203+1.232692+0.221674</f>
+        <v>3.6145690000000004</v>
       </c>
       <c r="G11" s="1">
         <f>B11-(E11+F11)</f>
-        <v>0.34153300000000009</v>
+        <v>36.482922999999992</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -4656,7 +4624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>

</xml_diff>